<commit_message>
office soft assertion implementation
</commit_message>
<xml_diff>
--- a/HybridFrameworkApr2019/src/test/resources/Sheets/SuiteA.xlsx
+++ b/HybridFrameworkApr2019/src/test/resources/Sheets/SuiteA.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="168" windowWidth="14808" windowHeight="7956" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="47">
   <si>
     <t>TCID</t>
   </si>
@@ -54,9 +54,6 @@
     <t>ExpectedResult</t>
   </si>
   <si>
-    <t>Mozilla</t>
-  </si>
-  <si>
     <t>U1</t>
   </si>
   <si>
@@ -157,12 +154,15 @@
   </si>
   <si>
     <t>loginButton_xpath</t>
+  </si>
+  <si>
+    <t>ProceedOnFail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -323,7 +323,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -358,7 +358,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -569,7 +569,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -627,10 +627,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -640,174 +640,214 @@
     <col min="3" max="3" width="20.88671875" customWidth="1"/>
     <col min="4" max="4" width="26.5546875" customWidth="1"/>
     <col min="5" max="5" width="21.44140625" customWidth="1"/>
+    <col min="6" max="6" width="13.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E3" s="5"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>42</v>
-      </c>
       <c r="E4" s="5"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E5" s="5"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E8" s="5"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E10" s="5"/>
+      <c r="F10" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E11" s="5"/>
+      <c r="F11" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E12" s="5"/>
+      <c r="F12" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -819,10 +859,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -859,16 +899,16 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -876,16 +916,16 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>17</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>18</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -893,125 +933,142 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
         <v>20</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>21</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="4" t="s">
+      <c r="C9" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
         <v>27</v>
       </c>
-      <c r="C10" t="s">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" t="s">
         <v>27</v>
-      </c>
-      <c r="C19" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>